<commit_message>
Add BiMap. Use Strings everywhere.
</commit_message>
<xml_diff>
--- a/data/OnlineRetailShort-Analyzed.xlsx
+++ b/data/OnlineRetailShort-Analyzed.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9060" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9060" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="OnlineRetailShort" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">OnlineRetailShort!$A$1:$K$100</definedName>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="381">
   <si>
     <t>InvoiceNo</t>
   </si>
@@ -1109,6 +1110,66 @@
   </si>
   <si>
     <t>(536378,21977)</t>
+  </si>
+  <si>
+    <t>(536378,11 24 51 14 38 4 71 22 17 15 1 54 61)</t>
+  </si>
+  <si>
+    <t>(536367,47 66 46 8 20 2 43 53 6 12 49 23)</t>
+  </si>
+  <si>
+    <t>(536376,59 3)</t>
+  </si>
+  <si>
+    <t>(536377,48 31)</t>
+  </si>
+  <si>
+    <t>(536366,31 48)</t>
+  </si>
+  <si>
+    <t>(536368,63 69 10 42)</t>
+  </si>
+  <si>
+    <t>(536365,41 70 60 37 26 68 28)</t>
+  </si>
+  <si>
+    <t>(536372,48 31)</t>
+  </si>
+  <si>
+    <t>(536373,41 70 60 44 36 29 21 72 50 57 18 25 37 26 68 28)</t>
+  </si>
+  <si>
+    <t>(536370,65 64 7 58 5 35 13 62 33 56 39 34 45 32 55 9 40 27 52 16)</t>
+  </si>
+  <si>
+    <t>(536375,41 70 60 44 36 29 21 72 50 57 18 25 37 26 68 28)</t>
+  </si>
+  <si>
+    <t>11 24 51 14 38 4 71 22 17 15 1 54 61</t>
+  </si>
+  <si>
+    <t>47 66 46 8 20 2 43 53 6 12 49 23</t>
+  </si>
+  <si>
+    <t>59 3</t>
+  </si>
+  <si>
+    <t>48 31</t>
+  </si>
+  <si>
+    <t>31 48</t>
+  </si>
+  <si>
+    <t>63 69 10 42</t>
+  </si>
+  <si>
+    <t>41 70 60 37 26 68 28</t>
+  </si>
+  <si>
+    <t>41 70 60 44 36 29 21 72 50 57 18 25 37 26 68 28</t>
+  </si>
+  <si>
+    <t>65 64 7 58 5 35 13 62 33 56 39 34 45 32 55 9 40 27 52 16</t>
   </si>
 </sst>
 </file>
@@ -1592,10 +1653,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5395,7 +5459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A72"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
@@ -5776,8 +5840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6582,4 +6646,160 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="55.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>379</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add count Unique. Add Main experiments
</commit_message>
<xml_diff>
--- a/data/OnlineRetailShort-Analyzed.xlsx
+++ b/data/OnlineRetailShort-Analyzed.xlsx
@@ -9,14 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9060" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9060" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="OnlineRetailShort" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
+    <sheet name="Unique items" sheetId="2" r:id="rId2"/>
+    <sheet name="Mapping" sheetId="3" r:id="rId3"/>
+    <sheet name="Pairs" sheetId="4" r:id="rId4"/>
+    <sheet name="Transactions" sheetId="5" r:id="rId5"/>
+    <sheet name="FPGrowth 0,2" sheetId="6" r:id="rId6"/>
+    <sheet name="FPGrowth 0,1" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">OnlineRetailShort!$A$1:$K$100</definedName>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="479">
   <si>
     <t>InvoiceNo</t>
   </si>
@@ -1170,6 +1172,300 @@
   </si>
   <si>
     <t>65 64 7 58 5 35 13 62 33 56 39 34 45 32 55 9 40 27 52 16</t>
+  </si>
+  <si>
+    <t>(84969,1)</t>
+  </si>
+  <si>
+    <t>(21733,1)</t>
+  </si>
+  <si>
+    <t>(84997C,1)</t>
+  </si>
+  <si>
+    <t>(21883,1)</t>
+  </si>
+  <si>
+    <t>(21754,1)</t>
+  </si>
+  <si>
+    <t>(22726,1)</t>
+  </si>
+  <si>
+    <t>(22749,1)</t>
+  </si>
+  <si>
+    <t>(21913,1)</t>
+  </si>
+  <si>
+    <t>(22912,1)</t>
+  </si>
+  <si>
+    <t>(22386,1)</t>
+  </si>
+  <si>
+    <t>(21755,1)</t>
+  </si>
+  <si>
+    <t>(21791,1)</t>
+  </si>
+  <si>
+    <t>(20723,1)</t>
+  </si>
+  <si>
+    <t>(22352,1)</t>
+  </si>
+  <si>
+    <t>(POST,1)</t>
+  </si>
+  <si>
+    <t>(21559,1)</t>
+  </si>
+  <si>
+    <t>(82482,2)</t>
+  </si>
+  <si>
+    <t>(21258,1)</t>
+  </si>
+  <si>
+    <t>(22310,1)</t>
+  </si>
+  <si>
+    <t>(21071,2)</t>
+  </si>
+  <si>
+    <t>(20725,1)</t>
+  </si>
+  <si>
+    <t>(48187,1)</t>
+  </si>
+  <si>
+    <t>(85099C,1)</t>
+  </si>
+  <si>
+    <t>(82494L,2)</t>
+  </si>
+  <si>
+    <t>(84029E,3)</t>
+  </si>
+  <si>
+    <t>(22544,1)</t>
+  </si>
+  <si>
+    <t>(21730,3)</t>
+  </si>
+  <si>
+    <t>(21871,2)</t>
+  </si>
+  <si>
+    <t>(22086,1)</t>
+  </si>
+  <si>
+    <t>(22633,3)</t>
+  </si>
+  <si>
+    <t>(21731,1)</t>
+  </si>
+  <si>
+    <t>(22326,1)</t>
+  </si>
+  <si>
+    <t>(22631,1)</t>
+  </si>
+  <si>
+    <t>(10002,1)</t>
+  </si>
+  <si>
+    <t>(37370,2)</t>
+  </si>
+  <si>
+    <t>(84029G,3)</t>
+  </si>
+  <si>
+    <t>(84997B,1)</t>
+  </si>
+  <si>
+    <t>(22659,1)</t>
+  </si>
+  <si>
+    <t>(22540,1)</t>
+  </si>
+  <si>
+    <t>(85123A,3)</t>
+  </si>
+  <si>
+    <t>(22914,1)</t>
+  </si>
+  <si>
+    <t>(22623,1)</t>
+  </si>
+  <si>
+    <t>(20679,2)</t>
+  </si>
+  <si>
+    <t>(22661,1)</t>
+  </si>
+  <si>
+    <t>(22748,1)</t>
+  </si>
+  <si>
+    <t>(84879,1)</t>
+  </si>
+  <si>
+    <t>(22632,3)</t>
+  </si>
+  <si>
+    <t>(21777,1)</t>
+  </si>
+  <si>
+    <t>(82483,2)</t>
+  </si>
+  <si>
+    <t>(21033,1)</t>
+  </si>
+  <si>
+    <t>(22492,1)</t>
+  </si>
+  <si>
+    <t>(22622,1)</t>
+  </si>
+  <si>
+    <t>(21975,1)</t>
+  </si>
+  <si>
+    <t>(22900,1)</t>
+  </si>
+  <si>
+    <t>(22629,1)</t>
+  </si>
+  <si>
+    <t>(82486,2)</t>
+  </si>
+  <si>
+    <t>(21724,1)</t>
+  </si>
+  <si>
+    <t>(22114,1)</t>
+  </si>
+  <si>
+    <t>(84406B,3)</t>
+  </si>
+  <si>
+    <t>(21977,1)</t>
+  </si>
+  <si>
+    <t>(21035,1)</t>
+  </si>
+  <si>
+    <t>(22960,1)</t>
+  </si>
+  <si>
+    <t>(22727,1)</t>
+  </si>
+  <si>
+    <t>(22728,1)</t>
+  </si>
+  <si>
+    <t>(22745,1)</t>
+  </si>
+  <si>
+    <t>(21756,1)</t>
+  </si>
+  <si>
+    <t>(22752,3)</t>
+  </si>
+  <si>
+    <t>(22913,1)</t>
+  </si>
+  <si>
+    <t>(71053,3)</t>
+  </si>
+  <si>
+    <t>(21094,1)</t>
+  </si>
+  <si>
+    <t>(21068,2)</t>
+  </si>
+  <si>
+    <t>22386 85099C 21033 20723 84997B 84997C 21094 20725 21559 22352 21212 21975 21977</t>
+  </si>
+  <si>
+    <t>84879 22745 22748 22749 22310 84969 22623 22622 21754 21755 21777 48187</t>
+  </si>
+  <si>
+    <t>22114 21733</t>
+  </si>
+  <si>
+    <t>22632 22633</t>
+  </si>
+  <si>
+    <t>22633 22632</t>
+  </si>
+  <si>
+    <t>22960 22913 22912 22914</t>
+  </si>
+  <si>
+    <t>85123A 71053 84406B 84029G 84029E 22752 21730</t>
+  </si>
+  <si>
+    <t>85123A 71053 84406B 20679 37370 21871 21071 21068 82483 82486 82482 82494L 84029G 84029E 22752 21730</t>
+  </si>
+  <si>
+    <t>22728 22727 22726 21724 21883 10002 21791 21035 22326 22629 22659 22631 22661 21731 22900 21913 22540 22544 22492 POST</t>
+  </si>
+  <si>
+    <t>{71053}: 3</t>
+  </si>
+  <si>
+    <t>{22633}: 3</t>
+  </si>
+  <si>
+    <t>{22632}: 3</t>
+  </si>
+  <si>
+    <t>{85123A}: 3</t>
+  </si>
+  <si>
+    <t>{22752}: 3</t>
+  </si>
+  <si>
+    <t>{21730}: 3</t>
+  </si>
+  <si>
+    <t>{84029G}: 3</t>
+  </si>
+  <si>
+    <t>{84406B}: 3</t>
+  </si>
+  <si>
+    <t>{84029E}: 3</t>
+  </si>
+  <si>
+    <t>{21068}: 2</t>
+  </si>
+  <si>
+    <t>{82494L}: 2</t>
+  </si>
+  <si>
+    <t>{20679}: 2</t>
+  </si>
+  <si>
+    <t>{37370}: 2</t>
+  </si>
+  <si>
+    <t>{82486}: 2</t>
+  </si>
+  <si>
+    <t>{21071}: 2</t>
+  </si>
+  <si>
+    <t>{82482}: 2</t>
+  </si>
+  <si>
+    <t>{21871}: 2</t>
+  </si>
+  <si>
+    <t>{82483}: 2</t>
   </si>
 </sst>
 </file>
@@ -2017,8 +2313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4854,602 +5150,819 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B73"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.28515625" customWidth="1"/>
     <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>10002</v>
       </c>
       <c r="B1">
         <v>10002</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20679</v>
       </c>
       <c r="B2">
         <v>20679</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20723</v>
       </c>
       <c r="B3">
         <v>20723</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20725</v>
       </c>
       <c r="B4">
         <v>20725</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>21033</v>
       </c>
       <c r="B5">
         <v>21033</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>21035</v>
       </c>
       <c r="B6">
         <v>21035</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>21068</v>
       </c>
       <c r="B7">
         <v>21068</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>21071</v>
       </c>
       <c r="B8">
         <v>21071</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>21094</v>
       </c>
       <c r="B9">
         <v>21094</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>21212</v>
       </c>
       <c r="B10">
         <v>21212</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>21258</v>
       </c>
       <c r="B11">
         <v>21258</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>21559</v>
       </c>
       <c r="B12">
         <v>21559</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>21724</v>
       </c>
       <c r="B13">
         <v>21724</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>21730</v>
       </c>
       <c r="B14">
         <v>21730</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>21731</v>
       </c>
       <c r="B15">
         <v>21731</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>21733</v>
       </c>
       <c r="B16">
         <v>21733</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>21754</v>
       </c>
       <c r="B17">
         <v>21754</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>21755</v>
       </c>
       <c r="B18">
         <v>21755</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>21756</v>
       </c>
       <c r="B19">
         <v>21756</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>21777</v>
       </c>
       <c r="B20">
         <v>21777</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>21791</v>
       </c>
       <c r="B21">
         <v>21791</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21871</v>
       </c>
       <c r="B22">
         <v>21871</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21883</v>
       </c>
       <c r="B23">
         <v>21883</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>21913</v>
       </c>
       <c r="B24">
         <v>21913</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>21975</v>
       </c>
       <c r="B25">
         <v>21975</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>21977</v>
       </c>
       <c r="B26">
         <v>21977</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>22086</v>
       </c>
       <c r="B27">
         <v>22086</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>22114</v>
       </c>
       <c r="B28">
         <v>22114</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>22310</v>
       </c>
       <c r="B29">
         <v>22310</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>22326</v>
       </c>
       <c r="B30">
         <v>22326</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>22352</v>
       </c>
       <c r="B31">
         <v>22352</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>22386</v>
       </c>
       <c r="B32">
         <v>22386</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>22492</v>
       </c>
       <c r="B33">
         <v>22492</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>22540</v>
       </c>
       <c r="B34">
         <v>22540</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>22544</v>
       </c>
       <c r="B35">
         <v>22544</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>22622</v>
       </c>
       <c r="B36">
         <v>22622</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>22623</v>
       </c>
       <c r="B37">
         <v>22623</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>22629</v>
       </c>
       <c r="B38">
         <v>22629</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>22631</v>
       </c>
       <c r="B39">
         <v>22631</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>22632</v>
       </c>
       <c r="B40">
         <v>22632</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>22633</v>
       </c>
       <c r="B41">
         <v>22633</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>22659</v>
       </c>
       <c r="B42">
         <v>22659</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>22661</v>
       </c>
       <c r="B43">
         <v>22661</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>22726</v>
       </c>
       <c r="B44">
         <v>22726</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>22727</v>
       </c>
       <c r="B45">
         <v>22727</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>22728</v>
       </c>
       <c r="B46">
         <v>22728</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>22745</v>
       </c>
       <c r="B47">
         <v>22745</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>22748</v>
       </c>
       <c r="B48">
         <v>22748</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>22749</v>
       </c>
       <c r="B49">
         <v>22749</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>22752</v>
       </c>
       <c r="B50">
         <v>22752</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>22900</v>
       </c>
       <c r="B51">
         <v>22900</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>22912</v>
       </c>
       <c r="B52">
         <v>22912</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>22913</v>
       </c>
       <c r="B53">
         <v>22913</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>22914</v>
       </c>
       <c r="B54">
         <v>22914</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>22960</v>
       </c>
       <c r="B55">
         <v>22960</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>37370</v>
       </c>
       <c r="B56">
         <v>37370</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>48187</v>
       </c>
       <c r="B57">
         <v>48187</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>71053</v>
       </c>
       <c r="B58">
         <v>71053</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>82482</v>
       </c>
       <c r="B59">
         <v>82482</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>82483</v>
       </c>
       <c r="B60">
         <v>82483</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>82486</v>
       </c>
       <c r="B61">
         <v>82486</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>84879</v>
       </c>
       <c r="B62">
         <v>84879</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>84969</v>
       </c>
       <c r="B63">
         <v>84969</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>70</v>
       </c>
       <c r="B64" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>16</v>
       </c>
       <c r="B65" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>14</v>
       </c>
       <c r="B66" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>12</v>
       </c>
       <c r="B67" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>80</v>
       </c>
       <c r="B68" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>82</v>
       </c>
       <c r="B69" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>76</v>
       </c>
       <c r="B70" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>8</v>
       </c>
       <c r="B71" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>8</v>
       </c>
       <c r="B72" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>59</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:A100">
-    <sortCondition ref="A1"/>
+  <sortState ref="C1:C72">
+    <sortCondition ref="C1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5459,7 +5972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A72"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
@@ -5840,8 +6353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6650,9 +7163,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A30"/>
+  <dimension ref="A1:A46"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:A46"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6799,7 +7314,251 @@
         <v>379</v>
       </c>
     </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>22086</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>21258</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>21756</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>459</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>464</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:A130">
+    <sortCondition ref="A103"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="101.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>472</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:A65540">
+    <sortCondition descending="1" ref="A65441"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>